<commit_message>
Tabla de actividades de la segunda entrega con controles y recursos asignados, tambien se sube acta f[014]
</commit_message>
<xml_diff>
--- a/Actividades/Proy01006/Tabla de recursos.xlsx
+++ b/Actividades/Proy01006/Tabla de recursos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ProyectoFinal2019-\Actividades\Proy01006\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA65E1-9A35-4176-9B5D-F5BA5DAE30FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="20730" windowHeight="11700"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t xml:space="preserve">Tabla de Recurso </t>
   </si>
@@ -189,13 +195,19 @@
     <t>Sdedit</t>
   </si>
   <si>
-    <t>Dbaccess</t>
+    <t>Emacs</t>
+  </si>
+  <si>
+    <t>S[18]</t>
+  </si>
+  <si>
+    <t>MS-Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -438,22 +450,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>301547</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>209551</xdr:rowOff>
+      <xdr:rowOff>93594</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:colOff>1483475</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1135009</xdr:rowOff>
+      <xdr:rowOff>1275522</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF24399D-ABF7-472F-902D-9A6B29B34906}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF24399D-ABF7-472F-902D-9A6B29B34906}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -469,14 +481,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4610100" y="209551"/>
-          <a:ext cx="1133475" cy="925458"/>
+          <a:off x="4741025" y="93594"/>
+          <a:ext cx="1181928" cy="1181928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -531,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -583,7 +594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -777,18 +788,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1051,21 +1062,21 @@
     </row>
     <row r="24" spans="1:3" ht="18.75">
       <c r="A24" s="7" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75">
       <c r="A25" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>50</v>
@@ -1073,30 +1084,36 @@
     </row>
     <row r="26" spans="1:3" ht="18.75">
       <c r="A26" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:3" ht="18.75">
+      <c r="A27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" thickBot="1">
+      <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="18.75">
       <c r="A29" s="4"/>
@@ -1119,16 +1136,21 @@
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="18.75">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="18.75">
       <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="18.75">
       <c r="A35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="18.75">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Gantt completo, tabla de actividades completo, acta F[018]
</commit_message>
<xml_diff>
--- a/Actividades/Proy01006/Tabla de recursos.xlsx
+++ b/Actividades/Proy01006/Tabla de recursos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01006\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\HUB\ProyectoFinal2019-\Actividades\Proy01006\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF2F07D-D8D8-4E4A-A657-CCB46A407D2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114F0D3A-84F6-46CF-A7E5-1503FE5C0DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11700" yWindow="0" windowWidth="8535" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t xml:space="preserve">Tabla de Recurso </t>
   </si>
@@ -196,6 +196,36 @@
   </si>
   <si>
     <t>MS-Project</t>
+  </si>
+  <si>
+    <t>S[18]</t>
+  </si>
+  <si>
+    <t>S[19]</t>
+  </si>
+  <si>
+    <t>S[20]</t>
+  </si>
+  <si>
+    <t>Herramientas de desarrollo web</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>Premier</t>
+  </si>
+  <si>
+    <t>Facundo Silvetti</t>
+  </si>
+  <si>
+    <t>P[05]</t>
+  </si>
+  <si>
+    <t>T[05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computadora personal de Facundo Silvetti </t>
   </si>
 </sst>
 </file>
@@ -249,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -357,9 +387,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -372,9 +400,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -387,6 +413,58 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -396,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,18 +488,23 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,36 +873,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="105.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="6"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="20.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -869,21 +952,21 @@
     </row>
     <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="7" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>49</v>
@@ -891,10 +974,10 @@
     </row>
     <row r="9" spans="1:4" ht="18.75">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>49</v>
@@ -902,10 +985,10 @@
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>49</v>
@@ -913,10 +996,10 @@
     </row>
     <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>49</v>
@@ -924,10 +1007,10 @@
     </row>
     <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>49</v>
@@ -935,10 +1018,10 @@
     </row>
     <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>49</v>
@@ -946,10 +1029,10 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>49</v>
@@ -957,10 +1040,10 @@
     </row>
     <row r="15" spans="1:4" ht="18.75">
       <c r="A15" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
@@ -968,10 +1051,10 @@
     </row>
     <row r="16" spans="1:4" ht="18.75">
       <c r="A16" s="7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>49</v>
@@ -979,10 +1062,10 @@
     </row>
     <row r="17" spans="1:3" ht="18.75">
       <c r="A17" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>49</v>
@@ -990,10 +1073,10 @@
     </row>
     <row r="18" spans="1:3" ht="18.75">
       <c r="A18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>49</v>
@@ -1001,10 +1084,10 @@
     </row>
     <row r="19" spans="1:3" ht="18.75">
       <c r="A19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>49</v>
@@ -1012,10 +1095,10 @@
     </row>
     <row r="20" spans="1:3" ht="18.75">
       <c r="A20" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>49</v>
@@ -1023,10 +1106,10 @@
     </row>
     <row r="21" spans="1:3" ht="18.75">
       <c r="A21" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>49</v>
@@ -1034,10 +1117,10 @@
     </row>
     <row r="22" spans="1:3" ht="18.75">
       <c r="A22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>49</v>
@@ -1045,10 +1128,10 @@
     </row>
     <row r="23" spans="1:3" ht="18.75">
       <c r="A23" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>49</v>
@@ -1056,84 +1139,139 @@
     </row>
     <row r="24" spans="1:3" ht="18.75">
       <c r="A24" s="7" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75">
       <c r="A25" s="7" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75">
       <c r="A26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75">
+      <c r="A27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.75">
+      <c r="A28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18.75">
+      <c r="A29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.75">
+      <c r="A30" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B30" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C30" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A27" s="9" t="s">
+    <row r="31" spans="1:3" ht="18.75">
+      <c r="A31" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B31" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C31" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="18.75">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="18.75">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" ht="18.75">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" ht="18.75">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+    <row r="32" spans="1:3" ht="19.5" thickBot="1">
+      <c r="A32" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="18.75">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="18.75">
-      <c r="A34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="18.75">
-      <c r="A35" s="2"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" ht="18.75">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="18.75">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" ht="18.75">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="18.75">
+      <c r="A39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="18.75">
+      <c r="A40" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>